<commit_message>
Update TP Biochimie Image A2 ~ Guillaume Gégo 23h20
</commit_message>
<xml_diff>
--- a/Dataframes Excel (.xlsx)/ADN.xlsx
+++ b/Dataframes Excel (.xlsx)/ADN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\VirtualBox VMs\SciViews Box 2020\shared\projects\TP-Bioch-BAB2-Q1\Dataframes Excel (.xlsx)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA4BACF-7370-4756-AA25-826C8461B141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E0E3CC-44D8-4488-9A2E-A1F3A1793D17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17835" yWindow="495" windowWidth="21600" windowHeight="11385" xr2:uid="{58E2A8D9-AE62-4847-B1C5-3548FF4B9A82}"/>
+    <workbookView xWindow="6285" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{58E2A8D9-AE62-4847-B1C5-3548FF4B9A82}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>

</xml_diff>